<commit_message>
ribbon and structure changes
</commit_message>
<xml_diff>
--- a/Oh58.geo.test.xlsx
+++ b/Oh58.geo.test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jens\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\other\Oh58lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61D4027-BAD3-49AB-B472-387C47739884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77EECAC-CDB1-4F05-8C15-60A6C319247D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11775" yWindow="3420" windowWidth="28455" windowHeight="17145" xr2:uid="{1E47FF39-5132-4998-AB20-69EC08C701B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1E47FF39-5132-4998-AB20-69EC08C701B7}"/>
   </bookViews>
   <sheets>
     <sheet name="MIS01" sheetId="1" r:id="rId1"/>
@@ -782,30 +782,30 @@
   <dimension ref="B2:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
@@ -825,7 +825,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
@@ -848,7 +848,7 @@
         <v>-348526,5665485276</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -871,7 +871,7 @@
         <v>-350661,7327268717</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
@@ -900,7 +900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
@@ -929,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
@@ -960,7 +960,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
@@ -983,7 +983,7 @@
         <v>-335015,74532336084</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>-334622,917450776</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>-342513,69303899957</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>14.3615833333333</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>25</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>-348526,5665485276</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>-348526,5665485276</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>29</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>30</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>31</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>-348351,196469371</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>34</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>35</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>36</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>14.365309999999999</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>37</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>38</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>39</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>40</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>41</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>42</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>43</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="5" t="s">
         <v>44</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="5" t="s">
         <v>45</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="5" t="s">
         <v>46</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="5" t="s">
         <v>47</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>48</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>49</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="5" t="s">
         <v>50</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="5" t="s">
         <v>51</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="5" t="s">
         <v>52</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="5" t="s">
         <v>53</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
         <v>54</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
         <v>55</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>56</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
         <v>57</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" s="5" t="s">
         <v>58</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
         <v>59</v>
       </c>

</xml_diff>